<commit_message>
button assignment changes; attempt fix to autonomous
</commit_message>
<xml_diff>
--- a/2024 Button Assignments.xlsx
+++ b/2024 Button Assignments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveharry/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveharry/FRC/FRC_2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F65647F-4A7F-6742-8B90-73BCC59E8A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ED32A3D-E95F-B84C-9F3E-53A56077A875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36460" yWindow="500" windowWidth="36260" windowHeight="17440" activeTab="1" xr2:uid="{B0E47F15-67FA-9348-91FB-9EF001FB6296}"/>
+    <workbookView xWindow="-36460" yWindow="500" windowWidth="36260" windowHeight="17440" xr2:uid="{B0E47F15-67FA-9348-91FB-9EF001FB6296}"/>
   </bookViews>
   <sheets>
     <sheet name="Xbox" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="61">
   <si>
     <t>Controller</t>
   </si>
@@ -119,18 +119,12 @@
     <t>B</t>
   </si>
   <si>
-    <t>Goto the SOURCE (not working yet).</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Goto the AMP (only partially working so far).</t>
-  </si>
-  <si>
     <t>Back</t>
   </si>
   <si>
@@ -200,12 +194,6 @@
     <t>Shoot the note (no arm motion)</t>
   </si>
   <si>
-    <t>Arm to the Full Up position</t>
-  </si>
-  <si>
-    <t>Arm to the fully down, intake position.</t>
-  </si>
-  <si>
     <t>Stop all motors.</t>
   </si>
   <si>
@@ -242,9 +230,6 @@
     <t>guide</t>
   </si>
   <si>
-    <t>score note in amp.</t>
-  </si>
-  <si>
     <t>pick up a note running the motors until note is detected.</t>
   </si>
   <si>
@@ -252,6 +237,12 @@
   </si>
   <si>
     <t>Slow driving mode.</t>
+  </si>
+  <si>
+    <t>Move the note backwards in the shooter to the climbing position</t>
+  </si>
+  <si>
+    <t>Run the shooter backwards.</t>
   </si>
 </sst>
 </file>
@@ -547,7 +538,7 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1763688" cy="264560"/>
+    <xdr:ext cx="513667" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="7" name="TextBox 6">
@@ -562,7 +553,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3943350" y="5226050"/>
-          <a:ext cx="1763688" cy="264560"/>
+          <a:ext cx="513667" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -595,21 +586,8 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Raise Arm/Shoot/Lower</a:t>
+            <a:t>Shoot</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Arm</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1014,7 +992,7 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="780855" cy="264560"/>
+    <xdr:ext cx="184731" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="15" name="TextBox 14">
@@ -1029,7 +1007,66 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4679950" y="5575300"/>
-          <a:ext cx="780855" cy="264560"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="661912" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D811D3F6-3720-EE4C-350D-848F0223D31A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4686300" y="6064250"/>
+          <a:ext cx="661912" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1062,21 +1099,8 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Lower</a:t>
+            <a:t>Unshoot</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Arm</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1085,17 +1109,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2095500</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>2336800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="750142" cy="264560"/>
+    <xdr:ext cx="812851" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="TextBox 15">
+        <xdr:cNvPr id="17" name="TextBox 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D811D3F6-3720-EE4C-350D-848F0223D31A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49658A94-D04D-ACD0-CA0C-8819F579228B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1103,8 +1127,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4686300" y="6064250"/>
-          <a:ext cx="750142" cy="264560"/>
+          <a:off x="4927600" y="5816600"/>
+          <a:ext cx="812851" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1137,69 +1161,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Raise Arm</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2336800</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="580865" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="TextBox 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49658A94-D04D-ACD0-CA0C-8819F579228B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4927600" y="5816600"/>
-          <a:ext cx="580865" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Source</a:t>
+            <a:t>AdjustNote</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1213,7 +1175,7 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="443135" cy="264560"/>
+    <xdr:ext cx="184731" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="18" name="TextBox 17">
@@ -1228,7 +1190,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4438650" y="5810250"/>
-          <a:ext cx="443135" cy="264560"/>
+          <a:ext cx="184731" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1255,14 +1217,11 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Amp</a:t>
-          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2679,8 +2638,8 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2750,7 +2709,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2764,7 +2723,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2775,10 +2734,10 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2789,10 +2748,10 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2800,13 +2759,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2814,13 +2770,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2828,13 +2781,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2842,13 +2795,13 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2856,13 +2809,13 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2870,13 +2823,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2884,13 +2837,13 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2898,13 +2851,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2912,13 +2865,13 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2926,13 +2879,13 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2940,13 +2893,13 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2954,13 +2907,13 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2968,13 +2921,13 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2982,13 +2935,13 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2996,7 +2949,7 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3016,7 +2969,7 @@
   </sheetPr>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F36" sqref="F36:G36"/>
     </sheetView>
   </sheetViews>
@@ -3044,13 +2997,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3080,7 +3033,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3102,7 +3055,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3124,7 +3077,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3162,7 +3115,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3176,7 +3129,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3364,13 +3317,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3400,7 +3353,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3414,7 +3367,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3436,7 +3389,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3482,7 +3435,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>